<commit_message>
add anemometer class for additional heights
</commit_message>
<xml_diff>
--- a/Configuration_template_phase3.xlsx
+++ b/Configuration_template_phase3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aearntsen/CFARSPhase3/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F31E0B67-7836-5347-99C0-BBAB09888F92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C6B7B2-6D2F-0D41-8204-6F7B85248C4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-72060" yWindow="2340" windowWidth="31340" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35800" yWindow="3700" windowWidth="34480" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration_template" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="299">
   <si>
     <t>Timestamp</t>
   </si>
@@ -915,6 +915,24 @@
   </si>
   <si>
     <t>set up with IFPEN to run WiSE?</t>
+  </si>
+  <si>
+    <t>No RSD</t>
+  </si>
+  <si>
+    <t>ZX firware version</t>
+  </si>
+  <si>
+    <t>Anemometer Height 4 (m) Class, optional</t>
+  </si>
+  <si>
+    <t>Anemometer Height 1 (m) Class, optional</t>
+  </si>
+  <si>
+    <t>Anemometer Height 2 (m) Class, optional</t>
+  </si>
+  <si>
+    <t>Anemometer Height 3 (m) Class, optional</t>
   </si>
 </sst>
 </file>
@@ -1050,15 +1068,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>15409</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>21364</xdr:rowOff>
+      <xdr:colOff>26452</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>164929</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>855485</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>114496</xdr:rowOff>
+      <xdr:colOff>866528</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>70322</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1087,8 +1105,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4214692" y="3450364"/>
-          <a:ext cx="4498229" cy="3141132"/>
+          <a:off x="5570278" y="4107451"/>
+          <a:ext cx="5147033" cy="3096958"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1099,16 +1117,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>19144</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>108573</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>494013</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>42312</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>841435</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>164351</xdr:rowOff>
+      <xdr:colOff>819348</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>98091</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1137,8 +1155,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5188791" y="5935632"/>
-          <a:ext cx="5122753" cy="3163543"/>
+          <a:off x="5540883" y="7364138"/>
+          <a:ext cx="5129248" cy="3059605"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1162,8 +1180,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="D1:D17" totalsRowShown="0">
-  <autoFilter ref="D1:D17" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="D1:D21" totalsRowShown="0">
+  <autoFilter ref="D1:D21" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
@@ -1174,8 +1192,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="E1:F17" totalsRowShown="0">
-  <autoFilter ref="E1:F17" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="E1:F21" totalsRowShown="0">
+  <autoFilter ref="E1:F21" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Selection"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="If Option Selection is Other, Note Here"/>
@@ -1496,7 +1514,7 @@
   <dimension ref="A1:M135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1737,6 +1755,9 @@
       <c r="E11">
         <v>1</v>
       </c>
+      <c r="H11" s="5" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1793,7 +1814,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>167</v>
       </c>
@@ -1801,28 +1822,45 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>275</v>
       </c>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>296</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>297</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>170</v>
       </c>
@@ -1830,7 +1868,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>171</v>
       </c>
@@ -1838,7 +1876,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>277</v>
       </c>
@@ -1846,42 +1884,42 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>178</v>
       </c>
@@ -2493,7 +2531,7 @@
           <x14:formula1>
             <xm:f>Metadata!$H$2:$H$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E11:E12</xm:sqref>
+          <xm:sqref>E11:E12 E18:E21</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
@@ -2551,7 +2589,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6618A7A9-AFEA-8445-88C9-0D1B7DECEBDD}">
           <x14:formula1>
-            <xm:f>RSD_Models!$A$1:$A$10</xm:f>
+            <xm:f>RSD_Models!$A$1:$A$11</xm:f>
           </x14:formula1>
           <xm:sqref>E8</xm:sqref>
         </x14:dataValidation>
@@ -3276,10 +3314,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3337,6 +3375,11 @@
         <v>290</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>293</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>